<commit_message>
fixed LEFT formula for non-string values
</commit_message>
<xml_diff>
--- a/test/test.xlsx
+++ b/test/test.xlsx
@@ -5,41 +5,58 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>fd</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>sss</t>
-  </si>
-  <si>
-    <t>ds</t>
-  </si>
-  <si>
-    <t>go to</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ddd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testVar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otherVar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">put</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
   </si>
 </sst>
 </file>
@@ -47,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="166" formatCode="MMM\ D&quot;, &quot;YY"/>
   </numFmts>
@@ -146,15 +163,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1:M2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -186,19 +203,19 @@
       </c>
       <c r="B2" s="0" t="n">
         <f aca="true">RAND()</f>
-        <v>0.632280744612217</v>
+        <v>0.211689851950117</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">B2</f>
-        <v>0.632280744612217</v>
+        <v>0.211689851950117</v>
       </c>
       <c r="D2" s="1" t="str">
         <f aca="false">TEXT(Sheet2!B1, "dd-mm-yyyy")</f>
-        <v>02-10-2015</v>
+        <v>31-05-2016</v>
       </c>
       <c r="E2" s="2" t="n">
         <f aca="true">TODAY()</f>
-        <v>42279</v>
+        <v>42521</v>
       </c>
       <c r="F2" s="0" t="str">
         <f aca="false">TEXT(23, "##")</f>
@@ -206,11 +223,31 @@
       </c>
       <c r="G2" s="1" t="n">
         <f aca="false">Sheet2!A1</f>
-        <v>0.632280744612217</v>
+        <v>0.211689851950117</v>
       </c>
       <c r="H2" s="1" t="n">
         <f aca="false">B2+Sheet2!A1</f>
-        <v>1.26456148922443</v>
+        <v>0.423379703900234</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">LEFT(RANDBETWEEN(100000, 200000), 4)</f>
+        <v>1125</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -232,22 +269,22 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="I1:M2 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
         <f aca="false">Sheet1!B2</f>
-        <v>0.632280744612217</v>
+        <v>0.211689851950117</v>
       </c>
       <c r="B1" s="1" t="n">
         <f aca="true">TODAY()</f>
-        <v>42279</v>
+        <v>42521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>